<commit_message>
thêm chức năng thây đổi mật khẩu
</commit_message>
<xml_diff>
--- a/BaoCao/Proj Congty/Book1.xlsx
+++ b/BaoCao/Proj Congty/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ProjCT\BaoCao\Proj Congty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D43C7DA5-40EF-4E21-A366-C5A15C1318D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19D3EA-09DB-4CA3-80F1-EA75752A3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E16A3B9-0643-47B4-ACAA-24F04F4E6123}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Chức năng</t>
   </si>
@@ -140,13 +140,7 @@
     <t>Thay đổi thông tin cá nhân</t>
   </si>
   <si>
-    <t>Không thể chỉnh sửa tên/email/mật khẩu sau khi đăng ký</t>
-  </si>
-  <si>
     <t>Cập nhật ảnh đại diện</t>
-  </si>
-  <si>
-    <t>Chỉ chọn khi đăng ký, không thay đổi được sau đó</t>
   </si>
   <si>
     <t>Quản lý người dùng (Admin)</t>
@@ -207,7 +201,15 @@
     <t>Mỗi user đã có lịch sử riêng biệt</t>
   </si>
   <si>
-    <t>Đã hoạt động được ở trang Lịch sử nhưng chưa link tới dashboard</t>
+    <t>Có thể đổi tên cuộc hội thoại ở dashboard và trang lịch sử</t>
+  </si>
+  <si>
+    <t>Đã có thể cập nhật ảnh đại diện ở thông tin user và lúc đăng ký 
+tài khoản</t>
+  </si>
+  <si>
+    <t>có thể đổi tên nhưng không lưu tên mới ở adminpage, chưa thây đổi 
+được mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -307,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -349,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4AFE66-041C-439D-B881-315580073659}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -754,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -812,145 +817,147 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" ht="28.8">
+      <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8">
+      <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8">
+      <c r="A22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="43.2">
-      <c r="A22" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3">

</xml_diff>

<commit_message>
có thể thây đổi tên ở trang thông tin cá nhân
</commit_message>
<xml_diff>
--- a/BaoCao/Proj Congty/Book1.xlsx
+++ b/BaoCao/Proj Congty/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ProjCT\BaoCao\Proj Congty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19D3EA-09DB-4CA3-80F1-EA75752A3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14A316A-BADD-4BCB-9CDB-16EFB6E13788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E16A3B9-0643-47B4-ACAA-24F04F4E6123}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Chức năng</t>
   </si>
@@ -210,6 +210,14 @@
   <si>
     <t>có thể đổi tên nhưng không lưu tên mới ở adminpage, chưa thây đổi 
 được mật khẩu</t>
+  </si>
+  <si>
+    <t>Xuống dòng ở khung gửi tin nhắn cho bot, 
+bot hiểu và nhận định dạng xuống dòng</t>
+  </si>
+  <si>
+    <t>Bot có thể hiểu và "thấy" được tin nhắn xuống dòng, có tổ hợp phím 
+shift + enter ở khung chat</t>
   </si>
 </sst>
 </file>
@@ -346,14 +354,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4AFE66-041C-439D-B881-315580073659}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -695,10 +703,10 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -824,7 +832,7 @@
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -835,7 +843,7 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -960,10 +968,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
+    <row r="24" spans="1:3" ht="43.2">
+      <c r="A24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1"/>

</xml_diff>